<commit_message>
Adding the results collected so far to the folder
</commit_message>
<xml_diff>
--- a/ResultsFromRemote/Results_2.xlsx
+++ b/ResultsFromRemote/Results_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B29344-3B24-492D-85BE-A3B34A91BD6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDB389F-B8B5-40B1-8119-4A266A85C2D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="185">
   <si>
     <t>SeedSet Size</t>
   </si>
@@ -584,6 +584,9 @@
   </si>
   <si>
     <t xml:space="preserve">629 770 1533 1720 4920 5144 5224 6003 7047 9412 </t>
+  </si>
+  <si>
+    <t>Gain</t>
   </si>
 </sst>
 </file>
@@ -742,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -759,9 +762,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -776,24 +776,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -806,8 +788,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,32 +1101,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" customWidth="1"/>
     <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -1123,31 +1140,35 @@
       <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="31" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="1" t="s">
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="N1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="32"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="31" t="s">
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="33"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C2" s="46"/>
       <c r="D2" s="2"/>
       <c r="E2" s="4"/>
       <c r="F2" s="2" t="s">
@@ -1165,139 +1186,172 @@
       <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="T2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="32">
         <v>5</v>
       </c>
       <c r="C3" s="6">
         <v>5</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="20">
         <v>2252</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="21">
         <v>26839904</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>24396096</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="22">
         <v>2076</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="21">
         <v>5</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="20">
         <v>24694271</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="22">
         <v>2126</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="22">
+        <f>((G3-J3)/G3)*100</f>
+        <v>-2.4084778420038537</v>
+      </c>
+      <c r="L3" s="21">
         <v>8</v>
       </c>
-      <c r="L3" s="26">
+      <c r="M3" s="23">
         <v>26752341</v>
       </c>
-      <c r="M3" s="23">
+      <c r="N3" s="20">
         <v>24336574</v>
       </c>
-      <c r="N3" s="25">
+      <c r="O3" s="22">
         <v>2102</v>
       </c>
-      <c r="O3" s="24">
+      <c r="P3" s="22">
+        <f>((G3-O3)/G3)*100</f>
+        <v>-1.2524084778420037</v>
+      </c>
+      <c r="Q3" s="21">
         <v>15</v>
       </c>
-      <c r="P3" s="23">
+      <c r="R3" s="20">
         <v>24305571</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="S3" s="22">
         <v>2098</v>
       </c>
-      <c r="R3" s="24">
+      <c r="T3" s="22">
+        <f>((G3-S3)/G3)*100</f>
+        <v>-1.0597302504816954</v>
+      </c>
+      <c r="U3" s="21">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="35"/>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="29"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="8">
         <v>10</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="24">
         <v>1649</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="25">
         <v>26808767</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="24">
         <v>23230211</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="26">
         <v>1538</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="25">
         <v>5</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="24">
         <v>23903958</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4" s="26">
         <v>1567</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="40">
+        <f t="shared" ref="K4:K14" si="0">((G4-J4)/G4)*100</f>
+        <v>-1.8855656697009102</v>
+      </c>
+      <c r="L4" s="25">
         <v>8</v>
       </c>
-      <c r="L4" s="30">
+      <c r="M4" s="27">
         <v>26762780</v>
       </c>
-      <c r="M4" s="27">
+      <c r="N4" s="24">
         <v>23267579</v>
       </c>
-      <c r="N4" s="29">
+      <c r="O4" s="26">
         <v>1545</v>
       </c>
-      <c r="O4" s="28">
+      <c r="P4" s="40">
+        <f t="shared" ref="P4:P14" si="1">((G4-O4)/G4)*100</f>
+        <v>-0.45513654096228867</v>
+      </c>
+      <c r="Q4" s="25">
         <v>14</v>
       </c>
-      <c r="P4" s="27">
+      <c r="R4" s="24">
         <v>23165281</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="S4" s="26">
         <v>1544</v>
       </c>
-      <c r="R4" s="28">
+      <c r="T4" s="40">
+        <f t="shared" ref="T4:T14" si="2">((G4-S4)/G4)*100</f>
+        <v>-0.39011703511053319</v>
+      </c>
+      <c r="U4" s="25">
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="35"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="29"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="8">
         <v>15</v>
       </c>
@@ -1310,7 +1364,7 @@
       <c r="F5" s="7">
         <v>22335160</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="14">
         <v>1398</v>
       </c>
       <c r="H5" s="8">
@@ -1319,37 +1373,49 @@
       <c r="I5" s="7">
         <v>23256306</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="14">
         <v>1433</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="40">
+        <f t="shared" si="0"/>
+        <v>-2.503576537911302</v>
+      </c>
+      <c r="L5" s="8">
         <v>8</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="11">
         <v>26762785</v>
       </c>
-      <c r="M5" s="7">
+      <c r="N5" s="7">
         <v>22384769</v>
       </c>
-      <c r="N5" s="17">
+      <c r="O5" s="14">
         <v>1404</v>
       </c>
-      <c r="O5" s="8">
+      <c r="P5" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.42918454935622319</v>
+      </c>
+      <c r="Q5" s="8">
         <v>14</v>
       </c>
-      <c r="P5" s="7">
+      <c r="R5" s="7">
         <v>22348461</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="S5" s="14">
         <v>1401</v>
       </c>
-      <c r="R5" s="8">
+      <c r="T5" s="40">
+        <f t="shared" si="2"/>
+        <v>-0.21459227467811159</v>
+      </c>
+      <c r="U5" s="8">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="29"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="4">
         <v>20</v>
       </c>
@@ -1374,34 +1440,46 @@
       <c r="J6" s="3">
         <v>1414</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="39">
+        <f t="shared" si="0"/>
+        <v>-5.2083333333333339</v>
+      </c>
+      <c r="L6" s="4">
         <v>7</v>
       </c>
-      <c r="L6" s="12">
+      <c r="M6" s="12">
         <v>26798719</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>21655958</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>1343</v>
       </c>
-      <c r="O6" s="4">
+      <c r="P6" s="40">
+        <f t="shared" si="1"/>
+        <v>7.4404761904761904E-2</v>
+      </c>
+      <c r="Q6" s="4">
         <v>11</v>
       </c>
-      <c r="P6" s="2">
+      <c r="R6" s="2">
         <v>21609186</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="S6" s="3">
         <v>1344</v>
       </c>
-      <c r="R6" s="4">
+      <c r="T6" s="40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U6" s="4">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30">
         <v>10</v>
       </c>
       <c r="C7" s="6">
@@ -1428,34 +1506,46 @@
       <c r="J7" s="9">
         <v>3567</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="22">
+        <f t="shared" si="0"/>
+        <v>-1.4216661927779357</v>
+      </c>
+      <c r="L7" s="6">
         <v>7</v>
       </c>
-      <c r="L7" s="10">
+      <c r="M7" s="10">
         <v>26780876</v>
       </c>
-      <c r="M7" s="9">
+      <c r="N7" s="9">
         <v>24308245</v>
       </c>
-      <c r="N7" s="9">
+      <c r="O7" s="9">
         <v>3540</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="22">
+        <f t="shared" si="1"/>
+        <v>-0.65396644867785048</v>
+      </c>
+      <c r="Q7" s="6">
         <v>11</v>
       </c>
-      <c r="P7" s="5">
+      <c r="R7" s="5">
         <v>24344786</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="S7" s="9">
         <v>3538</v>
       </c>
-      <c r="R7" s="6">
+      <c r="T7" s="22">
+        <f t="shared" si="2"/>
+        <v>-0.59709980096673299</v>
+      </c>
+      <c r="U7" s="6">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="40"/>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="8">
         <v>10</v>
       </c>
@@ -1468,7 +1558,7 @@
       <c r="F8" s="7">
         <v>23202768</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="14">
         <v>2875</v>
       </c>
       <c r="H8" s="8">
@@ -1477,37 +1567,49 @@
       <c r="I8" s="7">
         <v>23935397</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="14">
         <v>2950</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="40">
+        <f t="shared" si="0"/>
+        <v>-2.6086956521739131</v>
+      </c>
+      <c r="L8" s="8">
         <v>6</v>
       </c>
-      <c r="L8" s="11">
+      <c r="M8" s="11">
         <v>26834618</v>
       </c>
-      <c r="M8" s="17">
+      <c r="N8" s="14">
         <v>23197216</v>
       </c>
-      <c r="N8" s="17">
+      <c r="O8" s="14">
         <v>2873</v>
       </c>
-      <c r="O8" s="8">
+      <c r="P8" s="40">
+        <f t="shared" si="1"/>
+        <v>6.9565217391304349E-2</v>
+      </c>
+      <c r="Q8" s="8">
         <v>9</v>
       </c>
-      <c r="P8" s="7">
+      <c r="R8" s="7">
         <v>23256502</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="S8" s="14">
         <v>2881</v>
       </c>
-      <c r="R8" s="8">
+      <c r="T8" s="40">
+        <f t="shared" si="2"/>
+        <v>-0.20869565217391303</v>
+      </c>
+      <c r="U8" s="8">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="40"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="29"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1520,7 +1622,7 @@
       <c r="F9" s="7">
         <v>22374196</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="14">
         <v>2660</v>
       </c>
       <c r="H9" s="8">
@@ -1529,37 +1631,49 @@
       <c r="I9" s="7">
         <v>23243623</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="14">
         <v>2759</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="40">
+        <f t="shared" si="0"/>
+        <v>-3.7218045112781954</v>
+      </c>
+      <c r="L9" s="8">
         <v>6</v>
       </c>
-      <c r="L9" s="11">
+      <c r="M9" s="11">
         <v>26803498</v>
       </c>
-      <c r="M9" s="17">
+      <c r="N9" s="14">
         <v>22403453</v>
       </c>
-      <c r="N9" s="17">
+      <c r="O9" s="14">
         <v>2674</v>
       </c>
-      <c r="O9" s="8">
+      <c r="P9" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.52631578947368418</v>
+      </c>
+      <c r="Q9" s="8">
         <v>10</v>
       </c>
-      <c r="P9" s="7">
+      <c r="R9" s="7">
         <v>22328087</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="S9" s="14">
         <v>2656</v>
       </c>
-      <c r="R9" s="8">
+      <c r="T9" s="40">
+        <f t="shared" si="2"/>
+        <v>0.15037593984962408</v>
+      </c>
+      <c r="U9" s="8">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="40"/>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="29"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="8">
         <v>20</v>
       </c>
@@ -1572,7 +1686,7 @@
       <c r="F10" s="7">
         <v>21639400</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="14">
         <v>2492</v>
       </c>
       <c r="H10" s="8">
@@ -1581,182 +1695,714 @@
       <c r="I10" s="7">
         <v>23019665</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="14">
         <v>2648</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="39">
+        <f t="shared" si="0"/>
+        <v>-6.2600321027287329</v>
+      </c>
+      <c r="L10" s="8">
         <v>7</v>
       </c>
-      <c r="L10" s="11">
+      <c r="M10" s="11">
         <v>26809013</v>
       </c>
-      <c r="M10" s="17">
+      <c r="N10" s="14">
         <v>21642413</v>
       </c>
-      <c r="N10" s="17">
+      <c r="O10" s="14">
         <v>2500</v>
       </c>
-      <c r="O10" s="8">
+      <c r="P10" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.32102728731942215</v>
+      </c>
+      <c r="Q10" s="8">
         <v>10</v>
       </c>
-      <c r="P10" s="7">
+      <c r="R10" s="7">
         <v>21614818</v>
       </c>
-      <c r="Q10" s="17">
+      <c r="S10" s="14">
         <v>2495</v>
       </c>
-      <c r="R10" s="8">
+      <c r="T10" s="40">
+        <f t="shared" si="2"/>
+        <v>-0.1203852327447833</v>
+      </c>
+      <c r="U10" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="32">
         <v>10</v>
       </c>
       <c r="C11" s="6">
         <v>5</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="6"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="35"/>
+      <c r="D11" s="5">
+        <v>7229</v>
+      </c>
+      <c r="E11" s="6">
+        <v>52398833</v>
+      </c>
+      <c r="F11" s="5">
+        <v>47647355</v>
+      </c>
+      <c r="G11" s="9">
+        <v>6830</v>
+      </c>
+      <c r="H11" s="6">
+        <v>11</v>
+      </c>
+      <c r="I11" s="5">
+        <v>49035174</v>
+      </c>
+      <c r="J11" s="9">
+        <v>6939</v>
+      </c>
+      <c r="K11" s="22">
+        <f t="shared" si="0"/>
+        <v>-1.5959004392386529</v>
+      </c>
+      <c r="L11" s="6">
+        <v>12</v>
+      </c>
+      <c r="M11" s="10">
+        <v>52460792</v>
+      </c>
+      <c r="N11" s="9">
+        <v>47655472</v>
+      </c>
+      <c r="O11" s="9">
+        <v>6829</v>
+      </c>
+      <c r="P11" s="22">
+        <f t="shared" si="1"/>
+        <v>1.4641288433382138E-2</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>24</v>
+      </c>
+      <c r="R11" s="5">
+        <v>47600446</v>
+      </c>
+      <c r="S11" s="9">
+        <v>6822</v>
+      </c>
+      <c r="T11" s="22">
+        <f t="shared" si="2"/>
+        <v>0.1171303074670571</v>
+      </c>
+      <c r="U11" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="8">
         <v>10</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="35"/>
+      <c r="D12" s="7">
+        <v>5811</v>
+      </c>
+      <c r="E12" s="8">
+        <v>52410866</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44154315</v>
+      </c>
+      <c r="G12" s="14">
+        <v>5158</v>
+      </c>
+      <c r="H12" s="8">
+        <v>15</v>
+      </c>
+      <c r="I12" s="7">
+        <v>46347293</v>
+      </c>
+      <c r="J12" s="14">
+        <v>5399</v>
+      </c>
+      <c r="K12" s="40">
+        <f t="shared" si="0"/>
+        <v>-4.672353625436215</v>
+      </c>
+      <c r="L12" s="8">
+        <v>17</v>
+      </c>
+      <c r="M12" s="11">
+        <v>52402757</v>
+      </c>
+      <c r="N12" s="14">
+        <v>44198736</v>
+      </c>
+      <c r="O12" s="14">
+        <v>5179</v>
+      </c>
+      <c r="P12" s="40">
+        <f t="shared" si="1"/>
+        <v>-0.40713454827452494</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>31</v>
+      </c>
+      <c r="R12" s="7">
+        <v>44087845</v>
+      </c>
+      <c r="S12" s="14">
+        <v>5169</v>
+      </c>
+      <c r="T12" s="40">
+        <f t="shared" si="2"/>
+        <v>-0.21326095385808455</v>
+      </c>
+      <c r="U12" s="8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="8">
         <v>15</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="8"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="36"/>
+      <c r="D13" s="7">
+        <v>5655</v>
+      </c>
+      <c r="E13" s="8">
+        <v>52303971</v>
+      </c>
+      <c r="F13" s="7">
+        <v>41964961</v>
+      </c>
+      <c r="G13" s="14">
+        <v>4874</v>
+      </c>
+      <c r="H13" s="8">
+        <v>10</v>
+      </c>
+      <c r="I13" s="7">
+        <v>44877839</v>
+      </c>
+      <c r="J13" s="14">
+        <v>5120</v>
+      </c>
+      <c r="K13" s="40">
+        <f t="shared" si="0"/>
+        <v>-5.0471891670086171</v>
+      </c>
+      <c r="L13" s="8">
+        <v>12</v>
+      </c>
+      <c r="M13" s="11">
+        <v>52338573</v>
+      </c>
+      <c r="N13" s="14">
+        <v>41955471</v>
+      </c>
+      <c r="O13" s="14">
+        <v>4871</v>
+      </c>
+      <c r="P13" s="40">
+        <f t="shared" si="1"/>
+        <v>6.1551087402544113E-2</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>25</v>
+      </c>
+      <c r="R13" s="7">
+        <v>42068211</v>
+      </c>
+      <c r="S13" s="14">
+        <v>4873</v>
+      </c>
+      <c r="T13" s="40">
+        <f t="shared" si="2"/>
+        <v>2.051702913418137E-2</v>
+      </c>
+      <c r="U13" s="8">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="4">
         <v>20</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="20"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39">
+      <c r="D14" s="16">
+        <v>4482</v>
+      </c>
+      <c r="E14" s="17">
+        <v>52396333</v>
+      </c>
+      <c r="F14" s="16">
+        <v>40433546</v>
+      </c>
+      <c r="G14" s="18">
+        <v>3797</v>
+      </c>
+      <c r="H14" s="17">
+        <v>11</v>
+      </c>
+      <c r="I14" s="16">
+        <v>43207655</v>
+      </c>
+      <c r="J14" s="18">
+        <v>3952</v>
+      </c>
+      <c r="K14" s="39">
+        <f t="shared" si="0"/>
+        <v>-4.0821701343165655</v>
+      </c>
+      <c r="L14" s="17">
+        <v>14</v>
+      </c>
+      <c r="M14" s="19">
+        <v>52392084</v>
+      </c>
+      <c r="N14" s="3">
+        <v>40412212</v>
+      </c>
+      <c r="O14" s="3">
+        <v>3803</v>
+      </c>
+      <c r="P14" s="39">
+        <f t="shared" si="1"/>
+        <v>-0.15801948907031868</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>29</v>
+      </c>
+      <c r="R14" s="16">
+        <v>40381317</v>
+      </c>
+      <c r="S14" s="18">
+        <v>3802</v>
+      </c>
+      <c r="T14" s="39">
+        <f t="shared" si="2"/>
+        <v>-0.13168290755859888</v>
+      </c>
+      <c r="U14" s="17">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30">
         <v>15</v>
       </c>
       <c r="C15" s="6">
         <v>5</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="17"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="14"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="42"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="40"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="8"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="8">
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="8"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="29"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="4">
         <v>20</v>
       </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="4"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="32">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>17387</v>
+      </c>
+      <c r="E19" s="6">
+        <v>125584056</v>
+      </c>
+      <c r="F19" s="5">
+        <v>123164343</v>
+      </c>
+      <c r="G19" s="9">
+        <v>16376</v>
+      </c>
+      <c r="H19" s="6">
+        <v>7</v>
+      </c>
+      <c r="I19" s="5">
+        <v>123076703</v>
+      </c>
+      <c r="J19" s="9">
+        <v>15245</v>
+      </c>
+      <c r="K19" s="40">
+        <f t="shared" ref="K19:K22" si="3">((G19-J19)/G19)*100</f>
+        <v>6.9064484611626771</v>
+      </c>
+      <c r="L19" s="6">
+        <v>5</v>
+      </c>
+      <c r="M19" s="10">
+        <v>125635245</v>
+      </c>
+      <c r="N19" s="5">
+        <v>122805687</v>
+      </c>
+      <c r="O19" s="9">
+        <v>16369</v>
+      </c>
+      <c r="P19" s="40">
+        <f t="shared" ref="P19:P22" si="4">((G19-O19)/G19)*100</f>
+        <v>4.2745481191988274E-2</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>39</v>
+      </c>
+      <c r="R19" s="5">
+        <v>122512215</v>
+      </c>
+      <c r="S19" s="9">
+        <v>16358</v>
+      </c>
+      <c r="T19" s="40">
+        <f t="shared" ref="T19:T22" si="5">((G19-S19)/G19)*100</f>
+        <v>0.10991695163654128</v>
+      </c>
+      <c r="U19" s="6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" s="29"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="8">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7">
+        <v>14068</v>
+      </c>
+      <c r="E20" s="8">
+        <v>125611250</v>
+      </c>
+      <c r="F20" s="7">
+        <v>122274274</v>
+      </c>
+      <c r="G20" s="14">
+        <v>14089</v>
+      </c>
+      <c r="H20" s="8">
+        <v>5</v>
+      </c>
+      <c r="I20" s="7">
+        <v>122165616</v>
+      </c>
+      <c r="J20" s="14">
+        <v>13599</v>
+      </c>
+      <c r="K20" s="40">
+        <f t="shared" si="3"/>
+        <v>3.4778905529136206</v>
+      </c>
+      <c r="L20" s="8">
+        <v>4</v>
+      </c>
+      <c r="M20" s="11">
+        <v>125642763</v>
+      </c>
+      <c r="N20" s="7">
+        <v>121548214</v>
+      </c>
+      <c r="O20" s="14">
+        <v>12911</v>
+      </c>
+      <c r="P20" s="40">
+        <f t="shared" si="4"/>
+        <v>8.3611327986372341</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>33</v>
+      </c>
+      <c r="R20" s="7">
+        <v>120896438</v>
+      </c>
+      <c r="S20" s="14">
+        <v>12567</v>
+      </c>
+      <c r="T20" s="40">
+        <f t="shared" si="5"/>
+        <v>10.802753921499042</v>
+      </c>
+      <c r="U20" s="8">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="29"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="8">
+        <v>15</v>
+      </c>
+      <c r="D21" s="7">
+        <v>12693</v>
+      </c>
+      <c r="E21" s="8">
+        <v>125652103</v>
+      </c>
+      <c r="F21" s="7">
+        <v>121032653</v>
+      </c>
+      <c r="G21" s="14">
+        <v>12046</v>
+      </c>
+      <c r="H21" s="8">
+        <v>6</v>
+      </c>
+      <c r="I21" s="7">
+        <v>121048899</v>
+      </c>
+      <c r="J21" s="14">
+        <v>9878</v>
+      </c>
+      <c r="K21" s="40">
+        <f t="shared" si="3"/>
+        <v>17.997675576955004</v>
+      </c>
+      <c r="L21" s="8">
+        <v>4</v>
+      </c>
+      <c r="M21" s="11">
+        <v>125634123</v>
+      </c>
+      <c r="N21" s="7">
+        <v>120426167</v>
+      </c>
+      <c r="O21" s="14">
+        <v>10364</v>
+      </c>
+      <c r="P21" s="40">
+        <f t="shared" si="4"/>
+        <v>13.963141291715091</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>32</v>
+      </c>
+      <c r="R21" s="7">
+        <v>119459314</v>
+      </c>
+      <c r="S21" s="14">
+        <v>10509</v>
+      </c>
+      <c r="T21" s="40">
+        <f t="shared" si="5"/>
+        <v>12.759422214843102</v>
+      </c>
+      <c r="U21" s="8">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="29"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="4">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2">
+        <v>11704</v>
+      </c>
+      <c r="E22" s="4">
+        <v>125625700</v>
+      </c>
+      <c r="F22" s="2">
+        <v>120486327</v>
+      </c>
+      <c r="G22" s="3">
+        <v>10813</v>
+      </c>
+      <c r="H22" s="4">
+        <v>5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>120199966</v>
+      </c>
+      <c r="J22" s="3">
+        <v>10424</v>
+      </c>
+      <c r="K22" s="39">
+        <f t="shared" si="3"/>
+        <v>3.5975215018958657</v>
+      </c>
+      <c r="L22" s="4">
+        <v>4</v>
+      </c>
+      <c r="M22" s="12">
+        <v>125610793</v>
+      </c>
+      <c r="N22" s="2">
+        <v>119066537</v>
+      </c>
+      <c r="O22" s="3">
+        <v>9034</v>
+      </c>
+      <c r="P22" s="39">
+        <f t="shared" si="4"/>
+        <v>16.452418385276982</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>33</v>
+      </c>
+      <c r="R22" s="2">
+        <v>118131168</v>
+      </c>
+      <c r="S22" s="3">
+        <v>9057</v>
+      </c>
+      <c r="T22" s="40">
+        <f t="shared" si="5"/>
+        <v>16.239711458429667</v>
+      </c>
+      <c r="U22" s="4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="29"/>
+      <c r="B23" s="30">
+        <v>20</v>
+      </c>
+      <c r="C23" s="6">
+        <v>5</v>
+      </c>
+      <c r="T23" s="9"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A25" s="29"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A26" s="29"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="4">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="B3:B6"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="A11:A18"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="B15:B18"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B3:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1778,15 +2424,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1871,15 +2517,15 @@
       </c>
     </row>
     <row r="19" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="41" t="s">
+      <c r="F19" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1964,15 +2610,15 @@
       </c>
     </row>
     <row r="37" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="41" t="s">
+      <c r="F37" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -2057,15 +2703,15 @@
       </c>
     </row>
     <row r="55" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F55" s="41" t="s">
+      <c r="F55" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="G55" s="41"/>
-      <c r="H55" s="41"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="41"/>
-      <c r="K55" s="41"/>
-      <c r="L55" s="41"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="38"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -2150,15 +2796,15 @@
       </c>
     </row>
     <row r="73" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F73" s="41" t="s">
+      <c r="F73" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="G73" s="41"/>
-      <c r="H73" s="41"/>
-      <c r="I73" s="41"/>
-      <c r="J73" s="41"/>
-      <c r="K73" s="41"/>
-      <c r="L73" s="41"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="38"/>
+      <c r="L73" s="38"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -2243,15 +2889,15 @@
       </c>
     </row>
     <row r="91" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F91" s="41" t="s">
+      <c r="F91" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="G91" s="41"/>
-      <c r="H91" s="41"/>
-      <c r="I91" s="41"/>
-      <c r="J91" s="41"/>
-      <c r="K91" s="41"/>
-      <c r="L91" s="41"/>
+      <c r="G91" s="38"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="38"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="38"/>
+      <c r="L91" s="38"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
@@ -2336,15 +2982,15 @@
       </c>
     </row>
     <row r="109" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F109" s="41" t="s">
+      <c r="F109" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="G109" s="41"/>
-      <c r="H109" s="41"/>
-      <c r="I109" s="41"/>
-      <c r="J109" s="41"/>
-      <c r="K109" s="41"/>
-      <c r="L109" s="41"/>
+      <c r="G109" s="38"/>
+      <c r="H109" s="38"/>
+      <c r="I109" s="38"/>
+      <c r="J109" s="38"/>
+      <c r="K109" s="38"/>
+      <c r="L109" s="38"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
@@ -2429,15 +3075,15 @@
       </c>
     </row>
     <row r="127" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F127" s="41" t="s">
+      <c r="F127" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="G127" s="41"/>
-      <c r="H127" s="41"/>
-      <c r="I127" s="41"/>
-      <c r="J127" s="41"/>
-      <c r="K127" s="41"/>
-      <c r="L127" s="41"/>
+      <c r="G127" s="38"/>
+      <c r="H127" s="38"/>
+      <c r="I127" s="38"/>
+      <c r="J127" s="38"/>
+      <c r="K127" s="38"/>
+      <c r="L127" s="38"/>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">

</xml_diff>